<commit_message>
Added - Manager in excel generation and view report.
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Ching,Mark Angelo.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Ching,Mark Angelo.xlsx
@@ -627,7 +627,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="7" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -869,7 +869,7 @@
         <v>49</v>
       </c>
       <c r="E14" s="7" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>

</xml_diff>